<commit_message>
Update test baselines with reversed ROI order. Add more supported rtimagelabels
</commit_message>
<xml_diff>
--- a/test/data/roi_stats_baseline.xlsx
+++ b/test/data/roi_stats_baseline.xlsx
@@ -520,22 +520,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="1">
-        <v>1.051261398765697</v>
+        <v>1.051269787511679</v>
       </c>
       <c r="F2" s="1">
-        <v>1.051255886161194</v>
+        <v>1.051264741649434</v>
       </c>
       <c r="G2" s="1">
         <v>1.051339798850324</v>
       </c>
       <c r="H2" s="1">
-        <v>1.051264741649434</v>
+        <v>1.051255886161194</v>
       </c>
       <c r="I2" s="1">
-        <v>1.051269787511679</v>
+        <v>1.051261398765697</v>
       </c>
       <c r="J2" s="2">
-        <v>1.051278322587665</v>
+        <v>1.051278322587666</v>
       </c>
       <c r="K2" s="3">
         <v>7.982137387685384E-05</v>
@@ -555,19 +555,19 @@
         <v>25</v>
       </c>
       <c r="E3" s="1">
-        <v>0.04143825450274045</v>
+        <v>0.04141474386841633</v>
       </c>
       <c r="F3" s="1">
-        <v>0.04149362750598951</v>
+        <v>0.04144832607046804</v>
       </c>
       <c r="G3" s="1">
         <v>0.04148816340401185</v>
       </c>
       <c r="H3" s="1">
-        <v>0.04144832607046804</v>
+        <v>0.04149362750598951</v>
       </c>
       <c r="I3" s="1">
-        <v>0.04141474386841633</v>
+        <v>0.04143825450274045</v>
       </c>
       <c r="J3" s="2">
         <v>0.04145662307032523</v>
@@ -590,19 +590,19 @@
         <v>26</v>
       </c>
       <c r="E4" s="1">
-        <v>1.076680493837373</v>
+        <v>1.076726249501096</v>
       </c>
       <c r="F4" s="1">
-        <v>1.076090302763109</v>
+        <v>1.075989517135804</v>
       </c>
       <c r="G4" s="1">
         <v>1.077385920585414</v>
       </c>
       <c r="H4" s="1">
-        <v>1.075989517135804</v>
+        <v>1.076090302763109</v>
       </c>
       <c r="I4" s="1">
-        <v>1.076726249501096</v>
+        <v>1.076680493837373</v>
       </c>
       <c r="J4" s="2">
         <v>1.076574496764559</v>
@@ -625,22 +625,22 @@
         <v>26</v>
       </c>
       <c r="E5" s="1">
-        <v>0.04212464269667251</v>
+        <v>0.04206104918741712</v>
       </c>
       <c r="F5" s="1">
-        <v>0.04227474176203542</v>
+        <v>0.04206963080482708</v>
       </c>
       <c r="G5" s="1">
         <v>0.04249410510222455</v>
       </c>
       <c r="H5" s="1">
-        <v>0.04206963080482708</v>
+        <v>0.04227474176203542</v>
       </c>
       <c r="I5" s="1">
-        <v>0.04206104918741712</v>
+        <v>0.04212464269667251</v>
       </c>
       <c r="J5" s="2">
-        <v>0.04220483391063534</v>
+        <v>0.04220483391063533</v>
       </c>
       <c r="K5" s="3">
         <v>0.01029588950284621</v>
@@ -660,22 +660,22 @@
         <v>26</v>
       </c>
       <c r="E6" s="1">
-        <v>0.03912455267628841</v>
+        <v>0.03906382816143492</v>
       </c>
       <c r="F6" s="1">
-        <v>0.03928549644345396</v>
+        <v>0.03909855080820211</v>
       </c>
       <c r="G6" s="1">
         <v>0.03944186042373258</v>
       </c>
       <c r="H6" s="1">
-        <v>0.03909855080820211</v>
+        <v>0.03928549644345396</v>
       </c>
       <c r="I6" s="1">
-        <v>0.03906382816143492</v>
+        <v>0.03912455267628841</v>
       </c>
       <c r="J6" s="2">
-        <v>0.03920285770262239</v>
+        <v>0.0392028577026224</v>
       </c>
       <c r="K6" s="3">
         <v>0.009677296877699915</v>
@@ -695,19 +695,19 @@
         <v>25</v>
       </c>
       <c r="E7" s="1">
-        <v>0.03941765059707679</v>
+        <v>0.03939497202373111</v>
       </c>
       <c r="F7" s="1">
-        <v>0.0394705304885466</v>
+        <v>0.03942710568361271</v>
       </c>
       <c r="G7" s="1">
         <v>0.03946218287311161</v>
       </c>
       <c r="H7" s="1">
-        <v>0.03942710568361271</v>
+        <v>0.0394705304885466</v>
       </c>
       <c r="I7" s="1">
-        <v>0.03939497202373111</v>
+        <v>0.03941765059707679</v>
       </c>
       <c r="J7" s="2">
         <v>0.03943448833321576</v>

</xml_diff>